<commit_message>
working on running conventional ML models
</commit_message>
<xml_diff>
--- a/ml_analysis_results.xlsx
+++ b/ml_analysis_results.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley Lo\My Documents\Summer 2021 NSERC\ml_for_opvs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley Lo\Documents\Summer 2021 NSERC\ml_for_opvs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D0A138-F2C3-4BFF-9F5F-E3C7DEFBEF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80BF9FC-C949-4CF8-B5A7-7FD6A7341F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{89160D80-ECCB-4350-8EBA-80C0C1DD8511}"/>
+    <workbookView xWindow="3072" yWindow="3072" windowWidth="23040" windowHeight="12204" activeTab="2" xr2:uid="{89160D80-ECCB-4350-8EBA-80C0C1DD8511}"/>
   </bookViews>
   <sheets>
-    <sheet name="OPVs from Min et al." sheetId="1" r:id="rId1"/>
+    <sheet name="opv_results" sheetId="1" r:id="rId1"/>
+    <sheet name="electronic_opv_results" sheetId="2" r:id="rId2"/>
+    <sheet name="device_opv_results" sheetId="3" r:id="rId3"/>
+    <sheet name="impt_device_opv_results" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="36">
   <si>
     <t>Summary of Model vs. Data Representation</t>
   </si>
@@ -172,6 +175,9 @@
   <si>
     <t>~2500</t>
   </si>
+  <si>
+    <t>SMILES, etc.</t>
+  </si>
 </sst>
 </file>
 
@@ -303,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -366,6 +372,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -682,20 +697,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8006122-67A7-4469-ADD5-B623037ECCEC}">
-  <dimension ref="A1:BD35"/>
+  <dimension ref="A1:AV35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AK7" sqref="AK7"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="1" customWidth="1"/>
+    <col min="6" max="8" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.44140625" style="1" customWidth="1"/>
@@ -703,22 +718,20 @@
     <col min="13" max="13" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="21" width="6.77734375" style="1" customWidth="1"/>
-    <col min="22" max="25" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="6.77734375" style="1" customWidth="1"/>
-    <col min="28" max="28" width="11.77734375" style="1" customWidth="1"/>
-    <col min="29" max="29" width="13" style="1" customWidth="1"/>
-    <col min="30" max="33" width="6.77734375" style="1" customWidth="1"/>
-    <col min="34" max="34" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="37" width="6.77734375" style="1" customWidth="1"/>
-    <col min="38" max="38" width="8.88671875" style="1"/>
-    <col min="39" max="56" width="6.77734375" style="1" customWidth="1"/>
-    <col min="57" max="16384" width="8.88671875" style="1"/>
+    <col min="16" max="17" width="18.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="17.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20" style="1" customWidth="1"/>
+    <col min="27" max="27" width="14" style="1" customWidth="1"/>
+    <col min="28" max="29" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="48" width="6.77734375" style="1" customWidth="1"/>
+    <col min="49" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:48" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -818,30 +831,14 @@
       <c r="AG1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="AJ1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AL1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="AN1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="AO1" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
       <c r="AP1" s="2"/>
       <c r="AQ1" s="2"/>
       <c r="AR1" s="2"/>
@@ -849,16 +846,8 @@
       <c r="AT1" s="2"/>
       <c r="AU1" s="2"/>
       <c r="AV1" s="2"/>
-      <c r="AW1" s="2"/>
-      <c r="AX1" s="2"/>
-      <c r="AY1" s="2"/>
-      <c r="AZ1" s="2"/>
-      <c r="BA1" s="2"/>
-      <c r="BB1" s="2"/>
-      <c r="BC1" s="2"/>
-      <c r="BD1" s="2"/>
-    </row>
-    <row r="2" spans="1:56" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -911,77 +900,61 @@
         <v>12</v>
       </c>
       <c r="R2" s="21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S2" s="21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T2" s="21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U2" s="21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V2" s="21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="W2" s="21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="X2" s="21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Y2" s="21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Z2" s="21" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="AA2" s="21" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="AB2" s="21" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="AC2" s="21" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="AD2" s="21" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AE2" s="21" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AF2" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG2" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH2" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="AI2" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="AJ2" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="AK2" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="AL2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="AM2" s="21" t="s">
+      <c r="AG2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="AN2" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="AO2" s="21" t="s">
-        <v>18</v>
-      </c>
+      <c r="AH2" s="12"/>
+      <c r="AI2" s="12"/>
+      <c r="AJ2" s="12"/>
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="12"/>
+      <c r="AM2" s="12"/>
+      <c r="AN2" s="12"/>
+      <c r="AO2" s="12"/>
       <c r="AP2" s="12"/>
       <c r="AQ2" s="12"/>
       <c r="AR2" s="12"/>
@@ -989,16 +962,8 @@
       <c r="AT2" s="12"/>
       <c r="AU2" s="12"/>
       <c r="AV2" s="12"/>
-      <c r="AW2" s="12"/>
-      <c r="AX2" s="12"/>
-      <c r="AY2" s="12"/>
-      <c r="AZ2" s="12"/>
-      <c r="BA2" s="12"/>
-      <c r="BB2" s="12"/>
-      <c r="BC2" s="12"/>
-      <c r="BD2" s="12"/>
-    </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1051,77 +1016,61 @@
         <v>1.0180263540824099E-2</v>
       </c>
       <c r="R3" s="11">
-        <v>0.50517811574911797</v>
+        <v>0.51613149900019595</v>
       </c>
       <c r="S3" s="11">
-        <v>6.8668668716107606E-2</v>
+        <v>8.8052527986181697E-2</v>
       </c>
       <c r="T3" s="10">
-        <v>0.18120386720185999</v>
+        <v>0.179525541170931</v>
       </c>
       <c r="U3" s="10">
-        <v>1.2685762217853801E-2</v>
+        <v>1.6039509965260299E-2</v>
       </c>
       <c r="V3" s="11">
-        <v>0.48297155215684401</v>
+        <v>0.51812458842905895</v>
       </c>
       <c r="W3" s="11">
-        <v>8.6016822360077294E-2</v>
+        <v>8.3569494716285594E-2</v>
       </c>
       <c r="X3" s="10">
-        <v>0.18808186385825401</v>
+        <v>0.18044759672343999</v>
       </c>
       <c r="Y3" s="10">
-        <v>1.40797668616841E-2</v>
+        <v>1.58875281138996E-2</v>
       </c>
       <c r="Z3" s="11">
-        <v>0.51613149900019595</v>
+        <v>0.50336330316799305</v>
       </c>
       <c r="AA3" s="11">
-        <v>8.8052527986181697E-2</v>
+        <v>0.10812420181979</v>
       </c>
       <c r="AB3" s="10">
-        <v>0.179525541170931</v>
+        <v>0.186444534354122</v>
       </c>
       <c r="AC3" s="10">
-        <v>1.6039509965260299E-2</v>
+        <v>2.2105417703307401E-2</v>
       </c>
       <c r="AD3" s="11">
-        <v>0.51812458842905895</v>
+        <v>0.63779712363765595</v>
       </c>
       <c r="AE3" s="11">
-        <v>8.3569494716285594E-2</v>
+        <v>7.1580188319444293E-2</v>
       </c>
       <c r="AF3" s="10">
-        <v>0.18044759672343999</v>
+        <v>0.160867114945872</v>
       </c>
       <c r="AG3" s="10">
-        <v>1.58875281138996E-2</v>
-      </c>
-      <c r="AH3" s="11">
-        <v>0.50336330316799305</v>
-      </c>
-      <c r="AI3" s="11">
-        <v>0.10812420181979</v>
-      </c>
-      <c r="AJ3" s="10">
-        <v>0.186444534354122</v>
-      </c>
-      <c r="AK3" s="10">
-        <v>2.2105417703307401E-2</v>
-      </c>
-      <c r="AL3" s="11">
-        <v>0.63779712363765595</v>
-      </c>
-      <c r="AM3" s="11">
-        <v>7.1580188319444293E-2</v>
-      </c>
-      <c r="AN3" s="10">
-        <v>0.160867114945872</v>
-      </c>
-      <c r="AO3" s="10">
         <v>1.51569449836469E-2</v>
       </c>
+      <c r="AH3" s="13"/>
+      <c r="AI3" s="13"/>
+      <c r="AJ3" s="13"/>
+      <c r="AK3" s="13"/>
+      <c r="AL3" s="13"/>
+      <c r="AM3" s="13"/>
+      <c r="AN3" s="13"/>
+      <c r="AO3" s="13"/>
       <c r="AP3" s="13"/>
       <c r="AQ3" s="13"/>
       <c r="AR3" s="13"/>
@@ -1129,16 +1078,8 @@
       <c r="AT3" s="13"/>
       <c r="AU3" s="13"/>
       <c r="AV3" s="13"/>
-      <c r="AW3" s="13"/>
-      <c r="AX3" s="13"/>
-      <c r="AY3" s="13"/>
-      <c r="AZ3" s="13"/>
-      <c r="BA3" s="13"/>
-      <c r="BB3" s="13"/>
-      <c r="BC3" s="13"/>
-      <c r="BD3" s="13"/>
-    </row>
-    <row r="4" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -1191,77 +1132,61 @@
         <v>7.9834396019577893E-3</v>
       </c>
       <c r="R4" s="11">
-        <v>0.51629850840469904</v>
+        <v>0.52219801282162803</v>
       </c>
       <c r="S4" s="11">
-        <v>7.1572302763754703E-2</v>
+        <v>0.102505001089021</v>
       </c>
       <c r="T4" s="10">
-        <v>0.184125036001205</v>
+        <v>0.18265292048454199</v>
       </c>
       <c r="U4" s="10">
-        <v>1.5286094509065099E-2</v>
+        <v>2.0559933036565701E-2</v>
       </c>
       <c r="V4" s="11">
-        <v>0.47587069586765601</v>
+        <v>0.53054832197295998</v>
       </c>
       <c r="W4" s="11">
-        <v>5.82809238868938E-2</v>
+        <v>8.2040247355337298E-2</v>
       </c>
       <c r="X4" s="10">
-        <v>0.195469930768013</v>
+        <v>0.18308222293853699</v>
       </c>
       <c r="Y4" s="10">
-        <v>5.8509320951998199E-3</v>
+        <v>1.58132500946521E-2</v>
       </c>
       <c r="Z4" s="11">
-        <v>0.52219801282162803</v>
+        <v>0.49838487804055498</v>
       </c>
       <c r="AA4" s="11">
-        <v>0.102505001089021</v>
+        <v>7.1845280235151396E-2</v>
       </c>
       <c r="AB4" s="10">
-        <v>0.18265292048454199</v>
+        <v>0.19668415188789301</v>
       </c>
       <c r="AC4" s="10">
-        <v>2.0559933036565701E-2</v>
+        <v>2.0313398912549002E-2</v>
       </c>
       <c r="AD4" s="11">
-        <v>0.53054832197295998</v>
+        <v>0.62506070351312604</v>
       </c>
       <c r="AE4" s="11">
-        <v>8.2040247355337298E-2</v>
+        <v>7.6996073144885296E-2</v>
       </c>
       <c r="AF4" s="10">
-        <v>0.18308222293853699</v>
+        <v>0.16614349186420399</v>
       </c>
       <c r="AG4" s="10">
-        <v>1.58132500946521E-2</v>
-      </c>
-      <c r="AH4" s="11">
-        <v>0.49838487804055498</v>
-      </c>
-      <c r="AI4" s="11">
-        <v>7.1845280235151396E-2</v>
-      </c>
-      <c r="AJ4" s="10">
-        <v>0.19668415188789301</v>
-      </c>
-      <c r="AK4" s="10">
-        <v>2.0313398912549002E-2</v>
-      </c>
-      <c r="AL4" s="11">
-        <v>0.62506070351312604</v>
-      </c>
-      <c r="AM4" s="11">
-        <v>7.6996073144885296E-2</v>
-      </c>
-      <c r="AN4" s="10">
-        <v>0.16614349186420399</v>
-      </c>
-      <c r="AO4" s="10">
         <v>1.51354987174272E-2</v>
       </c>
+      <c r="AH4" s="13"/>
+      <c r="AI4" s="13"/>
+      <c r="AJ4" s="13"/>
+      <c r="AK4" s="13"/>
+      <c r="AL4" s="13"/>
+      <c r="AM4" s="13"/>
+      <c r="AN4" s="13"/>
+      <c r="AO4" s="13"/>
       <c r="AP4" s="13"/>
       <c r="AQ4" s="13"/>
       <c r="AR4" s="13"/>
@@ -1269,16 +1194,8 @@
       <c r="AT4" s="13"/>
       <c r="AU4" s="13"/>
       <c r="AV4" s="13"/>
-      <c r="AW4" s="13"/>
-      <c r="AX4" s="13"/>
-      <c r="AY4" s="13"/>
-      <c r="AZ4" s="13"/>
-      <c r="BA4" s="13"/>
-      <c r="BB4" s="13"/>
-      <c r="BC4" s="13"/>
-      <c r="BD4" s="13"/>
-    </row>
-    <row r="5" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -1331,77 +1248,61 @@
         <v>1.29864093754234E-2</v>
       </c>
       <c r="R5" s="11">
-        <v>0.44469038398412197</v>
+        <v>0.31909016597191903</v>
       </c>
       <c r="S5" s="11">
-        <v>0.128823004105521</v>
+        <v>9.2310729222128102E-2</v>
       </c>
       <c r="T5" s="10">
-        <v>0.18733564375460701</v>
+        <v>0.21758547874807899</v>
       </c>
       <c r="U5" s="10">
-        <v>1.6549159859917301E-2</v>
+        <v>3.7230471789902297E-2</v>
       </c>
       <c r="V5" s="11">
-        <v>0.34087187526315099</v>
+        <v>0.37892730161799199</v>
       </c>
       <c r="W5" s="11">
-        <v>0.11705410201871</v>
+        <v>0.124830415427801</v>
       </c>
       <c r="X5" s="10">
-        <v>0.25175498002220797</v>
+        <v>0.19467993722718199</v>
       </c>
       <c r="Y5" s="10">
-        <v>4.4739808434277099E-2</v>
+        <v>1.7571081819739199E-2</v>
       </c>
       <c r="Z5" s="11">
-        <v>0.31909016597191903</v>
+        <v>0.38794994538702798</v>
       </c>
       <c r="AA5" s="11">
-        <v>9.2310729222128102E-2</v>
+        <v>0.18037832810695301</v>
       </c>
       <c r="AB5" s="10">
-        <v>0.21758547874807899</v>
+        <v>0.20679652624185399</v>
       </c>
       <c r="AC5" s="10">
-        <v>3.7230471789902297E-2</v>
+        <v>2.88613549019077E-2</v>
       </c>
       <c r="AD5" s="11">
-        <v>0.37892730161799199</v>
+        <v>0.59437541597751198</v>
       </c>
       <c r="AE5" s="11">
-        <v>0.124830415427801</v>
+        <v>6.84953914291343E-2</v>
       </c>
       <c r="AF5" s="10">
-        <v>0.19467993722718199</v>
+        <v>0.16813545554378401</v>
       </c>
       <c r="AG5" s="10">
-        <v>1.7571081819739199E-2</v>
-      </c>
-      <c r="AH5" s="11">
-        <v>0.38794994538702798</v>
-      </c>
-      <c r="AI5" s="11">
-        <v>0.18037832810695301</v>
-      </c>
-      <c r="AJ5" s="10">
-        <v>0.20679652624185399</v>
-      </c>
-      <c r="AK5" s="10">
-        <v>2.88613549019077E-2</v>
-      </c>
-      <c r="AL5" s="11">
-        <v>0.59437541597751198</v>
-      </c>
-      <c r="AM5" s="11">
-        <v>6.84953914291343E-2</v>
-      </c>
-      <c r="AN5" s="10">
-        <v>0.16813545554378401</v>
-      </c>
-      <c r="AO5" s="10">
         <v>1.23984264086232E-2</v>
       </c>
+      <c r="AH5" s="13"/>
+      <c r="AI5" s="13"/>
+      <c r="AJ5" s="13"/>
+      <c r="AK5" s="13"/>
+      <c r="AL5" s="13"/>
+      <c r="AM5" s="13"/>
+      <c r="AN5" s="13"/>
+      <c r="AO5" s="13"/>
       <c r="AP5" s="13"/>
       <c r="AQ5" s="13"/>
       <c r="AR5" s="13"/>
@@ -1409,16 +1310,8 @@
       <c r="AT5" s="13"/>
       <c r="AU5" s="13"/>
       <c r="AV5" s="13"/>
-      <c r="AW5" s="13"/>
-      <c r="AX5" s="13"/>
-      <c r="AY5" s="13"/>
-      <c r="AZ5" s="13"/>
-      <c r="BA5" s="13"/>
-      <c r="BB5" s="13"/>
-      <c r="BC5" s="13"/>
-      <c r="BD5" s="13"/>
-    </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -1471,77 +1364,61 @@
         <v>1.9325895417603899E-2</v>
       </c>
       <c r="R6" s="11">
-        <v>0.13871448681904699</v>
+        <v>0.121833041998056</v>
       </c>
       <c r="S6" s="11">
-        <v>0.14887965450105201</v>
+        <v>8.0517441620664598E-2</v>
       </c>
       <c r="T6" s="10">
-        <v>0.31323367357254001</v>
+        <v>0.37120117545127801</v>
       </c>
       <c r="U6" s="10">
-        <v>4.0446217259314098E-2</v>
+        <v>2.74679535421672E-2</v>
       </c>
       <c r="V6" s="11">
-        <v>0.32848614912766599</v>
+        <v>0.25790425080519402</v>
       </c>
       <c r="W6" s="11">
-        <v>0.19459135986286399</v>
+        <v>0.12900217583704801</v>
       </c>
       <c r="X6" s="10">
-        <v>0.19661666154861401</v>
+        <v>0.37228112220764098</v>
       </c>
       <c r="Y6" s="10">
-        <v>2.2336285032396298E-2</v>
+        <v>3.6863792511377801E-2</v>
       </c>
       <c r="Z6" s="11">
-        <v>0.121833041998056</v>
+        <v>0.474695151891463</v>
       </c>
       <c r="AA6" s="11">
-        <v>8.0517441620664598E-2</v>
+        <v>7.51054881100299E-2</v>
       </c>
       <c r="AB6" s="10">
-        <v>0.37120117545127801</v>
+        <v>0.185158264636993</v>
       </c>
       <c r="AC6" s="10">
-        <v>2.74679535421672E-2</v>
+        <v>1.7660647702078602E-2</v>
       </c>
       <c r="AD6" s="11">
-        <v>0.25790425080519402</v>
+        <v>-4.3883100839761498E-2</v>
       </c>
       <c r="AE6" s="11">
-        <v>0.12900217583704801</v>
+        <v>0.10450753930880401</v>
       </c>
       <c r="AF6" s="10">
-        <v>0.37228112220764098</v>
+        <v>0.22812694013118701</v>
       </c>
       <c r="AG6" s="10">
-        <v>3.6863792511377801E-2</v>
-      </c>
-      <c r="AH6" s="11">
-        <v>0.474695151891463</v>
-      </c>
-      <c r="AI6" s="11">
-        <v>7.51054881100299E-2</v>
-      </c>
-      <c r="AJ6" s="10">
-        <v>0.185158264636993</v>
-      </c>
-      <c r="AK6" s="10">
-        <v>1.7660647702078602E-2</v>
-      </c>
-      <c r="AL6" s="11">
-        <v>-4.3883100839761498E-2</v>
-      </c>
-      <c r="AM6" s="11">
-        <v>0.10450753930880401</v>
-      </c>
-      <c r="AN6" s="10">
-        <v>0.22812694013118701</v>
-      </c>
-      <c r="AO6" s="10">
         <v>2.1164835993949398E-2</v>
       </c>
+      <c r="AH6" s="13"/>
+      <c r="AI6" s="13"/>
+      <c r="AJ6" s="13"/>
+      <c r="AK6" s="13"/>
+      <c r="AL6" s="13"/>
+      <c r="AM6" s="13"/>
+      <c r="AN6" s="13"/>
+      <c r="AO6" s="13"/>
       <c r="AP6" s="13"/>
       <c r="AQ6" s="13"/>
       <c r="AR6" s="13"/>
@@ -1549,16 +1426,8 @@
       <c r="AT6" s="13"/>
       <c r="AU6" s="13"/>
       <c r="AV6" s="13"/>
-      <c r="AW6" s="13"/>
-      <c r="AX6" s="13"/>
-      <c r="AY6" s="13"/>
-      <c r="AZ6" s="13"/>
-      <c r="BA6" s="13"/>
-      <c r="BB6" s="13"/>
-      <c r="BC6" s="13"/>
-      <c r="BD6" s="13"/>
-    </row>
-    <row r="7" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
@@ -1611,77 +1480,61 @@
         <v>1.5258345274574699E-2</v>
       </c>
       <c r="R7" s="11">
-        <v>0.43799156775841303</v>
+        <v>0.50262997945149701</v>
       </c>
       <c r="S7" s="11">
-        <v>9.6545600536255605E-2</v>
+        <v>0.16388825129094001</v>
       </c>
       <c r="T7" s="10">
-        <v>0.20039083361625601</v>
+        <v>0.195945584774017</v>
       </c>
       <c r="U7" s="10">
-        <v>2.9100933576306599E-2</v>
+        <v>2.9173049154102699E-2</v>
       </c>
       <c r="V7" s="11">
-        <v>0.53946479895176003</v>
+        <v>0.53531696123954498</v>
       </c>
       <c r="W7" s="11">
-        <v>0.158852154423125</v>
+        <v>0.11087596769201701</v>
       </c>
       <c r="X7" s="10">
-        <v>0.185461488366127</v>
+        <v>0.182043766975402</v>
       </c>
       <c r="Y7" s="10">
-        <v>3.9871449445618601E-2</v>
+        <v>3.0358750930346401E-2</v>
       </c>
       <c r="Z7" s="11">
-        <v>0.50262997945149701</v>
+        <v>0.58809799781212402</v>
       </c>
       <c r="AA7" s="11">
-        <v>0.16388825129094001</v>
+        <v>9.0978874010306604E-2</v>
       </c>
       <c r="AB7" s="10">
-        <v>0.195945584774017</v>
+        <v>0.178400143980979</v>
       </c>
       <c r="AC7" s="10">
-        <v>2.9173049154102699E-2</v>
+        <v>2.0484730652875399E-2</v>
       </c>
       <c r="AD7" s="11">
-        <v>0.53531696123954498</v>
+        <v>0.24710095478938099</v>
       </c>
       <c r="AE7" s="11">
-        <v>0.11087596769201701</v>
+        <v>0.20056195700301399</v>
       </c>
       <c r="AF7" s="10">
-        <v>0.182043766975402</v>
+        <v>0.20166546106338501</v>
       </c>
       <c r="AG7" s="10">
-        <v>3.0358750930346401E-2</v>
-      </c>
-      <c r="AH7" s="11">
-        <v>0.58809799781212402</v>
-      </c>
-      <c r="AI7" s="11">
-        <v>9.0978874010306604E-2</v>
-      </c>
-      <c r="AJ7" s="10">
-        <v>0.178400143980979</v>
-      </c>
-      <c r="AK7" s="10">
-        <v>2.0484730652875399E-2</v>
-      </c>
-      <c r="AL7" s="11">
-        <v>0.24710095478938099</v>
-      </c>
-      <c r="AM7" s="11">
-        <v>0.20056195700301399</v>
-      </c>
-      <c r="AN7" s="10">
-        <v>0.20166546106338501</v>
-      </c>
-      <c r="AO7" s="10">
         <v>1.02271487555842E-2</v>
       </c>
+      <c r="AH7" s="13"/>
+      <c r="AI7" s="13"/>
+      <c r="AJ7" s="13"/>
+      <c r="AK7" s="13"/>
+      <c r="AL7" s="13"/>
+      <c r="AM7" s="13"/>
+      <c r="AN7" s="13"/>
+      <c r="AO7" s="13"/>
       <c r="AP7" s="13"/>
       <c r="AQ7" s="13"/>
       <c r="AR7" s="13"/>
@@ -1689,16 +1542,8 @@
       <c r="AT7" s="13"/>
       <c r="AU7" s="13"/>
       <c r="AV7" s="13"/>
-      <c r="AW7" s="13"/>
-      <c r="AX7" s="13"/>
-      <c r="AY7" s="13"/>
-      <c r="AZ7" s="13"/>
-      <c r="BA7" s="13"/>
-      <c r="BB7" s="13"/>
-      <c r="BC7" s="13"/>
-      <c r="BD7" s="13"/>
-    </row>
-    <row r="8" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -1734,14 +1579,14 @@
       <c r="AE8" s="11"/>
       <c r="AF8" s="10"/>
       <c r="AG8" s="10"/>
-      <c r="AH8" s="11"/>
-      <c r="AI8" s="11"/>
-      <c r="AJ8" s="10"/>
-      <c r="AK8" s="10"/>
-      <c r="AL8" s="11"/>
-      <c r="AM8" s="11"/>
-      <c r="AN8" s="10"/>
-      <c r="AO8" s="10"/>
+      <c r="AH8" s="13"/>
+      <c r="AI8" s="13"/>
+      <c r="AJ8" s="13"/>
+      <c r="AK8" s="13"/>
+      <c r="AL8" s="13"/>
+      <c r="AM8" s="13"/>
+      <c r="AN8" s="13"/>
+      <c r="AO8" s="13"/>
       <c r="AP8" s="13"/>
       <c r="AQ8" s="13"/>
       <c r="AR8" s="13"/>
@@ -1749,16 +1594,8 @@
       <c r="AT8" s="13"/>
       <c r="AU8" s="13"/>
       <c r="AV8" s="13"/>
-      <c r="AW8" s="13"/>
-      <c r="AX8" s="13"/>
-      <c r="AY8" s="13"/>
-      <c r="AZ8" s="13"/>
-      <c r="BA8" s="13"/>
-      <c r="BB8" s="13"/>
-      <c r="BC8" s="13"/>
-      <c r="BD8" s="13"/>
-    </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>19</v>
       </c>
@@ -1794,16 +1631,8 @@
       <c r="AE9" s="14"/>
       <c r="AF9" s="14"/>
       <c r="AG9" s="14"/>
-      <c r="AH9" s="14"/>
-      <c r="AI9" s="14"/>
-      <c r="AJ9" s="14"/>
-      <c r="AK9" s="14"/>
-      <c r="AL9" s="14"/>
-      <c r="AM9" s="14"/>
-      <c r="AN9" s="14"/>
-      <c r="AO9" s="14"/>
-    </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>3</v>
       </c>
@@ -1839,16 +1668,8 @@
       <c r="AE10" s="11"/>
       <c r="AF10" s="10"/>
       <c r="AG10" s="10"/>
-      <c r="AH10" s="11"/>
-      <c r="AI10" s="11"/>
-      <c r="AJ10" s="10"/>
-      <c r="AK10" s="10"/>
-      <c r="AL10" s="11"/>
-      <c r="AM10" s="11"/>
-      <c r="AN10" s="10"/>
-      <c r="AO10" s="10"/>
-    </row>
-    <row r="11" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
@@ -1884,16 +1705,8 @@
       <c r="AE11" s="11"/>
       <c r="AF11" s="10"/>
       <c r="AG11" s="10"/>
-      <c r="AH11" s="11"/>
-      <c r="AI11" s="11"/>
-      <c r="AJ11" s="10"/>
-      <c r="AK11" s="10"/>
-      <c r="AL11" s="11"/>
-      <c r="AM11" s="11"/>
-      <c r="AN11" s="10"/>
-      <c r="AO11" s="10"/>
-    </row>
-    <row r="12" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
@@ -1929,16 +1742,8 @@
       <c r="AE12" s="11"/>
       <c r="AF12" s="10"/>
       <c r="AG12" s="10"/>
-      <c r="AH12" s="11"/>
-      <c r="AI12" s="11"/>
-      <c r="AJ12" s="10"/>
-      <c r="AK12" s="10"/>
-      <c r="AL12" s="11"/>
-      <c r="AM12" s="11"/>
-      <c r="AN12" s="10"/>
-      <c r="AO12" s="10"/>
-    </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
@@ -1974,16 +1779,8 @@
       <c r="AE13" s="11"/>
       <c r="AF13" s="10"/>
       <c r="AG13" s="10"/>
-      <c r="AH13" s="11"/>
-      <c r="AI13" s="11"/>
-      <c r="AJ13" s="10"/>
-      <c r="AK13" s="10"/>
-      <c r="AL13" s="11"/>
-      <c r="AM13" s="11"/>
-      <c r="AN13" s="10"/>
-      <c r="AO13" s="10"/>
-    </row>
-    <row r="14" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>7</v>
       </c>
@@ -2019,16 +1816,8 @@
       <c r="AE14" s="11"/>
       <c r="AF14" s="10"/>
       <c r="AG14" s="10"/>
-      <c r="AH14" s="11"/>
-      <c r="AI14" s="11"/>
-      <c r="AJ14" s="10"/>
-      <c r="AK14" s="10"/>
-      <c r="AL14" s="11"/>
-      <c r="AM14" s="11"/>
-      <c r="AN14" s="10"/>
-      <c r="AO14" s="10"/>
-    </row>
-    <row r="15" spans="1:56" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
@@ -2064,154 +1853,130 @@
       <c r="AE15" s="11"/>
       <c r="AF15" s="10"/>
       <c r="AG15" s="10"/>
-      <c r="AH15" s="11"/>
-      <c r="AI15" s="11"/>
-      <c r="AJ15" s="10"/>
-      <c r="AK15" s="10"/>
-      <c r="AL15" s="11"/>
-      <c r="AM15" s="11"/>
-      <c r="AN15" s="10"/>
-      <c r="AO15" s="10"/>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="17"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="Z21" s="18"/>
-      <c r="AA21" s="18"/>
-      <c r="AB21" s="18"/>
-      <c r="AC21" s="18"/>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="Z22" s="20"/>
-      <c r="AA22" s="20"/>
-      <c r="AB22" s="20"/>
-      <c r="AC22" s="20"/>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="Z23" s="19"/>
-      <c r="AA23" s="19"/>
-      <c r="AB23" s="19"/>
-      <c r="AC23" s="19"/>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="Z24" s="19"/>
-      <c r="AA24" s="19"/>
-      <c r="AB24" s="19"/>
-      <c r="AC24" s="19"/>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="Z25" s="19"/>
-      <c r="AA25" s="19"/>
-      <c r="AB25" s="19"/>
-      <c r="AC25" s="19"/>
-    </row>
-    <row r="26" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18"/>
+      <c r="U21" s="18"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="20"/>
+      <c r="U22" s="20"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R23" s="19"/>
+      <c r="S23" s="19"/>
+      <c r="T23" s="19"/>
+      <c r="U23" s="19"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="19"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="19"/>
+    </row>
+    <row r="26" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="6"/>
+      <c r="C26" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="D26" s="6" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G26" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="H26" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z26" s="19"/>
-      <c r="AA26" s="19"/>
-      <c r="AB26" s="19"/>
-      <c r="AC26" s="19"/>
-    </row>
-    <row r="27" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+    </row>
+    <row r="27" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B27" s="7">
         <v>386</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7">
+      <c r="C27" s="7">
         <v>386</v>
       </c>
+      <c r="D27" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="E27" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F27" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7">
+      <c r="F27" s="7">
         <v>386</v>
       </c>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7">
+      <c r="G27" s="7">
         <v>386</v>
       </c>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7" t="s">
+      <c r="H27" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7">
-        <v>386</v>
-      </c>
-      <c r="O27" s="7"/>
-      <c r="P27" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7">
-        <v>386</v>
-      </c>
-      <c r="Z27" s="19"/>
-      <c r="AA27" s="19"/>
-      <c r="AB27" s="19"/>
-      <c r="AC27" s="19"/>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="Z28" s="19"/>
-      <c r="AA28" s="19"/>
-      <c r="AB28" s="19"/>
-      <c r="AC28" s="19"/>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="Z29" s="18"/>
-      <c r="AA29" s="18"/>
-      <c r="AB29" s="18"/>
-      <c r="AC29" s="18"/>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R29" s="18"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="18"/>
+      <c r="U29" s="18"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>23</v>
       </c>
@@ -2219,12 +1984,12 @@
         <v>24</v>
       </c>
       <c r="C30" s="2"/>
-      <c r="Z30" s="19"/>
-      <c r="AA30" s="19"/>
-      <c r="AB30" s="19"/>
-      <c r="AC30" s="19"/>
-    </row>
-    <row r="31" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+    </row>
+    <row r="31" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>25</v>
       </c>
@@ -2235,37 +2000,3329 @@
       <c r="D31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Z31" s="19"/>
-      <c r="AA31" s="19"/>
-      <c r="AB31" s="19"/>
-      <c r="AC31" s="19"/>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="Z32" s="19"/>
-      <c r="AA32" s="19"/>
-      <c r="AB32" s="19"/>
-      <c r="AC32" s="19"/>
-    </row>
-    <row r="33" spans="26:29" x14ac:dyDescent="0.3">
-      <c r="Z33" s="19"/>
-      <c r="AA33" s="19"/>
-      <c r="AB33" s="19"/>
-      <c r="AC33" s="19"/>
-    </row>
-    <row r="34" spans="26:29" x14ac:dyDescent="0.3">
-      <c r="Z34" s="19"/>
-      <c r="AA34" s="19"/>
-      <c r="AB34" s="19"/>
-      <c r="AC34" s="19"/>
-    </row>
-    <row r="35" spans="26:29" x14ac:dyDescent="0.3">
-      <c r="Z35" s="19"/>
-      <c r="AA35" s="19"/>
-      <c r="AB35" s="19"/>
-      <c r="AC35" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="19"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+    </row>
+    <row r="33" spans="18:21" x14ac:dyDescent="0.3">
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="19"/>
+    </row>
+    <row r="34" spans="18:21" x14ac:dyDescent="0.3">
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+    </row>
+    <row r="35" spans="18:21" x14ac:dyDescent="0.3">
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="20" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE94539-DB0A-472C-B265-9C3EBD618CED}">
+  <dimension ref="A1:AV35"/>
+  <sheetViews>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.77734375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11.77734375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="13" style="1" customWidth="1"/>
+    <col min="22" max="25" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="6.77734375" style="1" customWidth="1"/>
+    <col min="30" max="30" width="8.88671875" style="1"/>
+    <col min="31" max="48" width="6.77734375" style="1" customWidth="1"/>
+    <col min="49" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:48" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+    </row>
+    <row r="2" spans="1:48" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="V2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="W2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="X2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH2" s="12"/>
+      <c r="AI2" s="12"/>
+      <c r="AJ2" s="12"/>
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="12"/>
+      <c r="AM2" s="12"/>
+      <c r="AN2" s="12"/>
+      <c r="AO2" s="12"/>
+      <c r="AP2" s="12"/>
+      <c r="AQ2" s="12"/>
+      <c r="AR2" s="12"/>
+      <c r="AS2" s="12"/>
+      <c r="AT2" s="12"/>
+      <c r="AU2" s="12"/>
+      <c r="AV2" s="12"/>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0.64019707781375501</v>
+      </c>
+      <c r="C3" s="11">
+        <v>5.7454559274925703E-2</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0.15359041845093599</v>
+      </c>
+      <c r="E3" s="10">
+        <v>1.1156571041259E-2</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0.64779420706744495</v>
+      </c>
+      <c r="G3" s="11">
+        <v>6.5917394838849494E-2</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0.15310024551714599</v>
+      </c>
+      <c r="I3" s="10">
+        <v>9.3276859194347302E-3</v>
+      </c>
+      <c r="J3" s="11">
+        <v>0.64848780945474105</v>
+      </c>
+      <c r="K3" s="11">
+        <v>5.8674020575526203E-2</v>
+      </c>
+      <c r="L3" s="10">
+        <v>0.15196405288224299</v>
+      </c>
+      <c r="M3" s="10">
+        <v>9.8987004567273797E-3</v>
+      </c>
+      <c r="N3" s="11">
+        <v>0.57104777853046396</v>
+      </c>
+      <c r="O3" s="11">
+        <v>7.2524323871029805E-2</v>
+      </c>
+      <c r="P3" s="10">
+        <v>0.166754952507843</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>9.28071818725173E-3</v>
+      </c>
+      <c r="R3" s="11">
+        <v>0.70022593270060196</v>
+      </c>
+      <c r="S3" s="11">
+        <v>6.7865905231643001E-2</v>
+      </c>
+      <c r="T3" s="10">
+        <v>0.14165081689268699</v>
+      </c>
+      <c r="U3" s="10">
+        <v>9.6826569767700706E-3</v>
+      </c>
+      <c r="V3" s="11">
+        <v>0.69799765338361097</v>
+      </c>
+      <c r="W3" s="11">
+        <v>7.3440678332130804E-2</v>
+      </c>
+      <c r="X3" s="10">
+        <v>0.14242627430007501</v>
+      </c>
+      <c r="Y3" s="10">
+        <v>1.1048918242824E-2</v>
+      </c>
+      <c r="Z3" s="11">
+        <v>0.62073101000284803</v>
+      </c>
+      <c r="AA3" s="11">
+        <v>0.11201511965437499</v>
+      </c>
+      <c r="AB3" s="10">
+        <v>0.15858274569848199</v>
+      </c>
+      <c r="AC3" s="10">
+        <v>1.6712764699067999E-2</v>
+      </c>
+      <c r="AD3" s="11">
+        <v>0.735927981000429</v>
+      </c>
+      <c r="AE3" s="11">
+        <v>4.24098231097974E-2</v>
+      </c>
+      <c r="AF3" s="10">
+        <v>0.13475517046942501</v>
+      </c>
+      <c r="AG3" s="10">
+        <v>1.11386073323601E-2</v>
+      </c>
+      <c r="AH3" s="13"/>
+      <c r="AI3" s="13"/>
+      <c r="AJ3" s="13"/>
+      <c r="AK3" s="13"/>
+      <c r="AL3" s="13"/>
+      <c r="AM3" s="13"/>
+      <c r="AN3" s="13"/>
+      <c r="AO3" s="13"/>
+      <c r="AP3" s="13"/>
+      <c r="AQ3" s="13"/>
+      <c r="AR3" s="13"/>
+      <c r="AS3" s="13"/>
+      <c r="AT3" s="13"/>
+      <c r="AU3" s="13"/>
+      <c r="AV3" s="13"/>
+    </row>
+    <row r="4" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="11"/>
+      <c r="AE4" s="11"/>
+      <c r="AF4" s="10"/>
+      <c r="AG4" s="10"/>
+      <c r="AH4" s="13"/>
+      <c r="AI4" s="13"/>
+      <c r="AJ4" s="13"/>
+      <c r="AK4" s="13"/>
+      <c r="AL4" s="13"/>
+      <c r="AM4" s="13"/>
+      <c r="AN4" s="13"/>
+      <c r="AO4" s="13"/>
+      <c r="AP4" s="13"/>
+      <c r="AQ4" s="13"/>
+      <c r="AR4" s="13"/>
+      <c r="AS4" s="13"/>
+      <c r="AT4" s="13"/>
+      <c r="AU4" s="13"/>
+      <c r="AV4" s="13"/>
+    </row>
+    <row r="5" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="11"/>
+      <c r="AE5" s="11"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="13"/>
+      <c r="AI5" s="13"/>
+      <c r="AJ5" s="13"/>
+      <c r="AK5" s="13"/>
+      <c r="AL5" s="13"/>
+      <c r="AM5" s="13"/>
+      <c r="AN5" s="13"/>
+      <c r="AO5" s="13"/>
+      <c r="AP5" s="13"/>
+      <c r="AQ5" s="13"/>
+      <c r="AR5" s="13"/>
+      <c r="AS5" s="13"/>
+      <c r="AT5" s="13"/>
+      <c r="AU5" s="13"/>
+      <c r="AV5" s="13"/>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="13"/>
+      <c r="AI6" s="13"/>
+      <c r="AJ6" s="13"/>
+      <c r="AK6" s="13"/>
+      <c r="AL6" s="13"/>
+      <c r="AM6" s="13"/>
+      <c r="AN6" s="13"/>
+      <c r="AO6" s="13"/>
+      <c r="AP6" s="13"/>
+      <c r="AQ6" s="13"/>
+      <c r="AR6" s="13"/>
+      <c r="AS6" s="13"/>
+      <c r="AT6" s="13"/>
+      <c r="AU6" s="13"/>
+      <c r="AV6" s="13"/>
+    </row>
+    <row r="7" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="11"/>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="10"/>
+      <c r="AH7" s="13"/>
+      <c r="AI7" s="13"/>
+      <c r="AJ7" s="13"/>
+      <c r="AK7" s="13"/>
+      <c r="AL7" s="13"/>
+      <c r="AM7" s="13"/>
+      <c r="AN7" s="13"/>
+      <c r="AO7" s="13"/>
+      <c r="AP7" s="13"/>
+      <c r="AQ7" s="13"/>
+      <c r="AR7" s="13"/>
+      <c r="AS7" s="13"/>
+      <c r="AT7" s="13"/>
+      <c r="AU7" s="13"/>
+      <c r="AV7" s="13"/>
+    </row>
+    <row r="8" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="11"/>
+      <c r="AE8" s="11"/>
+      <c r="AF8" s="10"/>
+      <c r="AG8" s="10"/>
+      <c r="AH8" s="13"/>
+      <c r="AI8" s="13"/>
+      <c r="AJ8" s="13"/>
+      <c r="AK8" s="13"/>
+      <c r="AL8" s="13"/>
+      <c r="AM8" s="13"/>
+      <c r="AN8" s="13"/>
+      <c r="AO8" s="13"/>
+      <c r="AP8" s="13"/>
+      <c r="AQ8" s="13"/>
+      <c r="AR8" s="13"/>
+      <c r="AS8" s="13"/>
+      <c r="AT8" s="13"/>
+      <c r="AU8" s="13"/>
+      <c r="AV8" s="13"/>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="14"/>
+      <c r="AB9" s="14"/>
+      <c r="AC9" s="14"/>
+      <c r="AD9" s="14"/>
+      <c r="AE9" s="14"/>
+      <c r="AF9" s="14"/>
+      <c r="AG9" s="14"/>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="10"/>
+      <c r="AC10" s="10"/>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="11"/>
+      <c r="AF10" s="10"/>
+      <c r="AG10" s="10"/>
+    </row>
+    <row r="11" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="10"/>
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="11"/>
+      <c r="AE11" s="11"/>
+      <c r="AF11" s="10"/>
+      <c r="AG11" s="10"/>
+    </row>
+    <row r="12" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="10"/>
+      <c r="AC12" s="10"/>
+      <c r="AD12" s="11"/>
+      <c r="AE12" s="11"/>
+      <c r="AF12" s="10"/>
+      <c r="AG12" s="10"/>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="10"/>
+      <c r="AC13" s="10"/>
+      <c r="AD13" s="11"/>
+      <c r="AE13" s="11"/>
+      <c r="AF13" s="10"/>
+      <c r="AG13" s="10"/>
+    </row>
+    <row r="14" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="10"/>
+      <c r="AC14" s="10"/>
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="11"/>
+      <c r="AF14" s="10"/>
+      <c r="AG14" s="10"/>
+    </row>
+    <row r="15" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="10"/>
+      <c r="AC15" s="10"/>
+      <c r="AD15" s="11"/>
+      <c r="AE15" s="11"/>
+      <c r="AF15" s="10"/>
+      <c r="AG15" s="10"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18"/>
+      <c r="U21" s="18"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="20"/>
+      <c r="U22" s="20"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R23" s="19"/>
+      <c r="S23" s="19"/>
+      <c r="T23" s="19"/>
+      <c r="U23" s="19"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="19"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="19"/>
+    </row>
+    <row r="26" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+    </row>
+    <row r="27" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R29" s="18"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="18"/>
+      <c r="U29" s="18"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+    </row>
+    <row r="31" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="19"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+    </row>
+    <row r="33" spans="18:21" x14ac:dyDescent="0.3">
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="19"/>
+    </row>
+    <row r="34" spans="18:21" x14ac:dyDescent="0.3">
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+    </row>
+    <row r="35" spans="18:21" x14ac:dyDescent="0.3">
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090AA089-3AF0-4715-92F8-6DE6C93BD25F}">
+  <dimension ref="A1:AV35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AG7" sqref="AG7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.77734375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="13" style="1" customWidth="1"/>
+    <col min="22" max="25" width="6.77734375" style="1" customWidth="1"/>
+    <col min="26" max="26" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="6.77734375" style="1" customWidth="1"/>
+    <col min="30" max="30" width="8.88671875" style="1"/>
+    <col min="31" max="48" width="6.77734375" style="1" customWidth="1"/>
+    <col min="49" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:48" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+    </row>
+    <row r="2" spans="1:48" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="V2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="W2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="X2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH2" s="12"/>
+      <c r="AI2" s="12"/>
+      <c r="AJ2" s="12"/>
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="12"/>
+      <c r="AM2" s="12"/>
+      <c r="AN2" s="12"/>
+      <c r="AO2" s="12"/>
+      <c r="AP2" s="12"/>
+      <c r="AQ2" s="12"/>
+      <c r="AR2" s="12"/>
+      <c r="AS2" s="12"/>
+      <c r="AT2" s="12"/>
+      <c r="AU2" s="12"/>
+      <c r="AV2" s="12"/>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0.34070619534164398</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0.15440717537027801</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0.123076200711825</v>
+      </c>
+      <c r="E3" s="10">
+        <v>2.1151676985403201E-2</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0.40041399472584399</v>
+      </c>
+      <c r="G3" s="11">
+        <v>0.396922961096566</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0.108932368405395</v>
+      </c>
+      <c r="I3" s="10">
+        <v>1.8105809306606501E-2</v>
+      </c>
+      <c r="J3" s="11">
+        <v>0.38162584139244699</v>
+      </c>
+      <c r="K3" s="11">
+        <v>0.13367077652852999</v>
+      </c>
+      <c r="L3" s="10">
+        <v>0.122828717817572</v>
+      </c>
+      <c r="M3" s="10">
+        <v>2.1108272640736801E-2</v>
+      </c>
+      <c r="N3" s="11">
+        <v>0.376855108789862</v>
+      </c>
+      <c r="O3" s="11">
+        <v>0.194906592946471</v>
+      </c>
+      <c r="P3" s="10">
+        <v>0.12846344194312401</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>2.0561367171827601E-2</v>
+      </c>
+      <c r="R3" s="11">
+        <v>0.39761035815252599</v>
+      </c>
+      <c r="S3" s="11">
+        <v>0.26778126526026003</v>
+      </c>
+      <c r="T3" s="10">
+        <v>0.12309441922915</v>
+      </c>
+      <c r="U3" s="10">
+        <v>1.9664648037731498E-2</v>
+      </c>
+      <c r="V3" s="11">
+        <v>0.38852529151653498</v>
+      </c>
+      <c r="W3" s="11">
+        <v>0.209482533719349</v>
+      </c>
+      <c r="X3" s="10">
+        <v>0.12333358716059301</v>
+      </c>
+      <c r="Y3" s="10">
+        <v>1.34152303186422E-2</v>
+      </c>
+      <c r="Z3" s="11">
+        <v>0.41449990645227702</v>
+      </c>
+      <c r="AA3" s="11">
+        <v>0.22765982541226601</v>
+      </c>
+      <c r="AB3" s="10">
+        <v>0.12934002360310501</v>
+      </c>
+      <c r="AC3" s="10">
+        <v>2.8735950442307801E-2</v>
+      </c>
+      <c r="AD3" s="11">
+        <v>0.45407344336669903</v>
+      </c>
+      <c r="AE3" s="11">
+        <v>0.27069625068716602</v>
+      </c>
+      <c r="AF3" s="10">
+        <v>0.120240471268413</v>
+      </c>
+      <c r="AG3" s="10">
+        <v>2.0261925889611499E-2</v>
+      </c>
+      <c r="AH3" s="13"/>
+      <c r="AI3" s="13"/>
+      <c r="AJ3" s="13"/>
+      <c r="AK3" s="13"/>
+      <c r="AL3" s="13"/>
+      <c r="AM3" s="13"/>
+      <c r="AN3" s="13"/>
+      <c r="AO3" s="13"/>
+      <c r="AP3" s="13"/>
+      <c r="AQ3" s="13"/>
+      <c r="AR3" s="13"/>
+      <c r="AS3" s="13"/>
+      <c r="AT3" s="13"/>
+      <c r="AU3" s="13"/>
+      <c r="AV3" s="13"/>
+    </row>
+    <row r="4" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0.334730888515334</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0.15826027061792</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.124129529203464</v>
+      </c>
+      <c r="E4" s="10">
+        <v>2.0751094628409499E-2</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0.42350359940982102</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0.37429957601791702</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0.107733192609829</v>
+      </c>
+      <c r="I4" s="10">
+        <v>1.8861413421736199E-2</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0.37781127817701599</v>
+      </c>
+      <c r="K4" s="11">
+        <v>0.133497695992111</v>
+      </c>
+      <c r="L4" s="10">
+        <v>0.123054169202758</v>
+      </c>
+      <c r="M4" s="10">
+        <v>2.1248355312088199E-2</v>
+      </c>
+      <c r="N4" s="11">
+        <v>0.38011304000577401</v>
+      </c>
+      <c r="O4" s="11">
+        <v>0.194985767687231</v>
+      </c>
+      <c r="P4" s="10">
+        <v>0.12817892723244401</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>2.02323993924255E-2</v>
+      </c>
+      <c r="R4" s="11">
+        <v>0.39719652011134698</v>
+      </c>
+      <c r="S4" s="11">
+        <v>0.26766076594699101</v>
+      </c>
+      <c r="T4" s="10">
+        <v>0.123171717728445</v>
+      </c>
+      <c r="U4" s="10">
+        <v>1.9654117251307598E-2</v>
+      </c>
+      <c r="V4" s="11">
+        <v>0.38856316359831</v>
+      </c>
+      <c r="W4" s="11">
+        <v>0.20949508500285199</v>
+      </c>
+      <c r="X4" s="10">
+        <v>0.12332873623827301</v>
+      </c>
+      <c r="Y4" s="10">
+        <v>1.3421266255906001E-2</v>
+      </c>
+      <c r="Z4" s="11">
+        <v>0.41510747450699098</v>
+      </c>
+      <c r="AA4" s="11">
+        <v>0.23021176502575399</v>
+      </c>
+      <c r="AB4" s="10">
+        <v>0.12920668543909999</v>
+      </c>
+      <c r="AC4" s="10">
+        <v>2.8738634791026601E-2</v>
+      </c>
+      <c r="AD4" s="11">
+        <v>0.46504711449744801</v>
+      </c>
+      <c r="AE4" s="11">
+        <v>0.269345466803044</v>
+      </c>
+      <c r="AF4" s="10">
+        <v>0.119633399730131</v>
+      </c>
+      <c r="AG4" s="10">
+        <v>1.9511758320773401E-2</v>
+      </c>
+      <c r="AH4" s="13"/>
+      <c r="AI4" s="13"/>
+      <c r="AJ4" s="13"/>
+      <c r="AK4" s="13"/>
+      <c r="AL4" s="13"/>
+      <c r="AM4" s="13"/>
+      <c r="AN4" s="13"/>
+      <c r="AO4" s="13"/>
+      <c r="AP4" s="13"/>
+      <c r="AQ4" s="13"/>
+      <c r="AR4" s="13"/>
+      <c r="AS4" s="13"/>
+      <c r="AT4" s="13"/>
+      <c r="AU4" s="13"/>
+      <c r="AV4" s="13"/>
+    </row>
+    <row r="5" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0.37248988967291202</v>
+      </c>
+      <c r="C5" s="11">
+        <v>0.24244148032555399</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.12201096085793001</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1.6569375090406499E-2</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0.30988887563614698</v>
+      </c>
+      <c r="G5" s="11">
+        <v>0.154352433521215</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0.12627876819568901</v>
+      </c>
+      <c r="I5" s="10">
+        <v>2.1440541943409198E-2</v>
+      </c>
+      <c r="J5" s="11">
+        <v>0.36517407700485799</v>
+      </c>
+      <c r="K5" s="11">
+        <v>0.20373004310526399</v>
+      </c>
+      <c r="L5" s="10">
+        <v>0.124775915105659</v>
+      </c>
+      <c r="M5" s="10">
+        <v>1.97513214902541E-2</v>
+      </c>
+      <c r="N5" s="11">
+        <v>0.44214982231773697</v>
+      </c>
+      <c r="O5" s="11">
+        <v>0.16509273954753101</v>
+      </c>
+      <c r="P5" s="10">
+        <v>0.12082679257603</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>1.6873802276520199E-2</v>
+      </c>
+      <c r="R5" s="11">
+        <v>0.19336858464161799</v>
+      </c>
+      <c r="S5" s="11">
+        <v>0.121030291954928</v>
+      </c>
+      <c r="T5" s="10">
+        <v>0.13534515810033201</v>
+      </c>
+      <c r="U5" s="10">
+        <v>2.16077055132698E-2</v>
+      </c>
+      <c r="V5" s="11">
+        <v>0.18159013932823201</v>
+      </c>
+      <c r="W5" s="11">
+        <v>0.19658608681957401</v>
+      </c>
+      <c r="X5" s="10">
+        <v>0.14153375345684699</v>
+      </c>
+      <c r="Y5" s="10">
+        <v>1.36785584632591E-2</v>
+      </c>
+      <c r="Z5" s="11">
+        <v>1.6487553924775199E-3</v>
+      </c>
+      <c r="AA5" s="11">
+        <v>0.11738964836103399</v>
+      </c>
+      <c r="AB5" s="10">
+        <v>0.202714698425255</v>
+      </c>
+      <c r="AC5" s="10">
+        <v>4.5671479669606899E-2</v>
+      </c>
+      <c r="AD5" s="11">
+        <v>0.32200527099083098</v>
+      </c>
+      <c r="AE5" s="11">
+        <v>0.22646544622477799</v>
+      </c>
+      <c r="AF5" s="10">
+        <v>0.13288722895878599</v>
+      </c>
+      <c r="AG5" s="10">
+        <v>1.9001758850667599E-2</v>
+      </c>
+      <c r="AH5" s="13"/>
+      <c r="AI5" s="13"/>
+      <c r="AJ5" s="13"/>
+      <c r="AK5" s="13"/>
+      <c r="AL5" s="13"/>
+      <c r="AM5" s="13"/>
+      <c r="AN5" s="13"/>
+      <c r="AO5" s="13"/>
+      <c r="AP5" s="13"/>
+      <c r="AQ5" s="13"/>
+      <c r="AR5" s="13"/>
+      <c r="AS5" s="13"/>
+      <c r="AT5" s="13"/>
+      <c r="AU5" s="13"/>
+      <c r="AV5" s="13"/>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="13"/>
+      <c r="AI6" s="13"/>
+      <c r="AJ6" s="13"/>
+      <c r="AK6" s="13"/>
+      <c r="AL6" s="13"/>
+      <c r="AM6" s="13"/>
+      <c r="AN6" s="13"/>
+      <c r="AO6" s="13"/>
+      <c r="AP6" s="13"/>
+      <c r="AQ6" s="13"/>
+      <c r="AR6" s="13"/>
+      <c r="AS6" s="13"/>
+      <c r="AT6" s="13"/>
+      <c r="AU6" s="13"/>
+      <c r="AV6" s="13"/>
+    </row>
+    <row r="7" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="11"/>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="10"/>
+      <c r="AH7" s="13"/>
+      <c r="AI7" s="13"/>
+      <c r="AJ7" s="13"/>
+      <c r="AK7" s="13"/>
+      <c r="AL7" s="13"/>
+      <c r="AM7" s="13"/>
+      <c r="AN7" s="13"/>
+      <c r="AO7" s="13"/>
+      <c r="AP7" s="13"/>
+      <c r="AQ7" s="13"/>
+      <c r="AR7" s="13"/>
+      <c r="AS7" s="13"/>
+      <c r="AT7" s="13"/>
+      <c r="AU7" s="13"/>
+      <c r="AV7" s="13"/>
+    </row>
+    <row r="8" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="11"/>
+      <c r="AE8" s="11"/>
+      <c r="AF8" s="10"/>
+      <c r="AG8" s="10"/>
+      <c r="AH8" s="13"/>
+      <c r="AI8" s="13"/>
+      <c r="AJ8" s="13"/>
+      <c r="AK8" s="13"/>
+      <c r="AL8" s="13"/>
+      <c r="AM8" s="13"/>
+      <c r="AN8" s="13"/>
+      <c r="AO8" s="13"/>
+      <c r="AP8" s="13"/>
+      <c r="AQ8" s="13"/>
+      <c r="AR8" s="13"/>
+      <c r="AS8" s="13"/>
+      <c r="AT8" s="13"/>
+      <c r="AU8" s="13"/>
+      <c r="AV8" s="13"/>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="14"/>
+      <c r="AB9" s="14"/>
+      <c r="AC9" s="14"/>
+      <c r="AD9" s="14"/>
+      <c r="AE9" s="14"/>
+      <c r="AF9" s="14"/>
+      <c r="AG9" s="14"/>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="10"/>
+      <c r="AC10" s="10"/>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="11"/>
+      <c r="AF10" s="10"/>
+      <c r="AG10" s="10"/>
+    </row>
+    <row r="11" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="10"/>
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="11"/>
+      <c r="AE11" s="11"/>
+      <c r="AF11" s="10"/>
+      <c r="AG11" s="10"/>
+    </row>
+    <row r="12" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="10"/>
+      <c r="AC12" s="10"/>
+      <c r="AD12" s="11"/>
+      <c r="AE12" s="11"/>
+      <c r="AF12" s="10"/>
+      <c r="AG12" s="10"/>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="10"/>
+      <c r="AC13" s="10"/>
+      <c r="AD13" s="11"/>
+      <c r="AE13" s="11"/>
+      <c r="AF13" s="10"/>
+      <c r="AG13" s="10"/>
+    </row>
+    <row r="14" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="10"/>
+      <c r="AC14" s="10"/>
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="11"/>
+      <c r="AF14" s="10"/>
+      <c r="AG14" s="10"/>
+    </row>
+    <row r="15" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="10"/>
+      <c r="AC15" s="10"/>
+      <c r="AD15" s="11"/>
+      <c r="AE15" s="11"/>
+      <c r="AF15" s="10"/>
+      <c r="AG15" s="10"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18"/>
+      <c r="U21" s="18"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="20"/>
+      <c r="U22" s="20"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R23" s="19"/>
+      <c r="S23" s="19"/>
+      <c r="T23" s="19"/>
+      <c r="U23" s="19"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="19"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="19"/>
+    </row>
+    <row r="26" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+    </row>
+    <row r="27" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R29" s="18"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="18"/>
+      <c r="U29" s="18"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+    </row>
+    <row r="31" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="19"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+    </row>
+    <row r="33" spans="18:21" x14ac:dyDescent="0.3">
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="19"/>
+    </row>
+    <row r="34" spans="18:21" x14ac:dyDescent="0.3">
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+    </row>
+    <row r="35" spans="18:21" x14ac:dyDescent="0.3">
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3639FAA3-E59D-43DC-813D-27DA78ACF0F0}">
+  <dimension ref="A1:AV35"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z8" sqref="Z8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="6.77734375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11.77734375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="13" style="1" customWidth="1"/>
+    <col min="22" max="25" width="6.77734375" style="1" customWidth="1"/>
+    <col min="26" max="26" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="6.77734375" style="1" customWidth="1"/>
+    <col min="30" max="30" width="8.88671875" style="1"/>
+    <col min="31" max="48" width="6.77734375" style="1" customWidth="1"/>
+    <col min="49" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:48" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+    </row>
+    <row r="2" spans="1:48" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="V2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="W2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="X2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH2" s="12"/>
+      <c r="AI2" s="12"/>
+      <c r="AJ2" s="12"/>
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="12"/>
+      <c r="AM2" s="12"/>
+      <c r="AN2" s="12"/>
+      <c r="AO2" s="12"/>
+      <c r="AP2" s="12"/>
+      <c r="AQ2" s="12"/>
+      <c r="AR2" s="12"/>
+      <c r="AS2" s="12"/>
+      <c r="AT2" s="12"/>
+      <c r="AU2" s="12"/>
+      <c r="AV2" s="12"/>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="11"/>
+      <c r="AE3" s="11"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="10"/>
+      <c r="AH3" s="13"/>
+      <c r="AI3" s="13"/>
+      <c r="AJ3" s="13"/>
+      <c r="AK3" s="13"/>
+      <c r="AL3" s="13"/>
+      <c r="AM3" s="13"/>
+      <c r="AN3" s="13"/>
+      <c r="AO3" s="13"/>
+      <c r="AP3" s="13"/>
+      <c r="AQ3" s="13"/>
+      <c r="AR3" s="13"/>
+      <c r="AS3" s="13"/>
+      <c r="AT3" s="13"/>
+      <c r="AU3" s="13"/>
+      <c r="AV3" s="13"/>
+    </row>
+    <row r="4" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="11"/>
+      <c r="AE4" s="11"/>
+      <c r="AF4" s="10"/>
+      <c r="AG4" s="10"/>
+      <c r="AH4" s="13"/>
+      <c r="AI4" s="13"/>
+      <c r="AJ4" s="13"/>
+      <c r="AK4" s="13"/>
+      <c r="AL4" s="13"/>
+      <c r="AM4" s="13"/>
+      <c r="AN4" s="13"/>
+      <c r="AO4" s="13"/>
+      <c r="AP4" s="13"/>
+      <c r="AQ4" s="13"/>
+      <c r="AR4" s="13"/>
+      <c r="AS4" s="13"/>
+      <c r="AT4" s="13"/>
+      <c r="AU4" s="13"/>
+      <c r="AV4" s="13"/>
+    </row>
+    <row r="5" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="11"/>
+      <c r="AE5" s="11"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="13"/>
+      <c r="AI5" s="13"/>
+      <c r="AJ5" s="13"/>
+      <c r="AK5" s="13"/>
+      <c r="AL5" s="13"/>
+      <c r="AM5" s="13"/>
+      <c r="AN5" s="13"/>
+      <c r="AO5" s="13"/>
+      <c r="AP5" s="13"/>
+      <c r="AQ5" s="13"/>
+      <c r="AR5" s="13"/>
+      <c r="AS5" s="13"/>
+      <c r="AT5" s="13"/>
+      <c r="AU5" s="13"/>
+      <c r="AV5" s="13"/>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="13"/>
+      <c r="AI6" s="13"/>
+      <c r="AJ6" s="13"/>
+      <c r="AK6" s="13"/>
+      <c r="AL6" s="13"/>
+      <c r="AM6" s="13"/>
+      <c r="AN6" s="13"/>
+      <c r="AO6" s="13"/>
+      <c r="AP6" s="13"/>
+      <c r="AQ6" s="13"/>
+      <c r="AR6" s="13"/>
+      <c r="AS6" s="13"/>
+      <c r="AT6" s="13"/>
+      <c r="AU6" s="13"/>
+      <c r="AV6" s="13"/>
+    </row>
+    <row r="7" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="11"/>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="10"/>
+      <c r="AH7" s="13"/>
+      <c r="AI7" s="13"/>
+      <c r="AJ7" s="13"/>
+      <c r="AK7" s="13"/>
+      <c r="AL7" s="13"/>
+      <c r="AM7" s="13"/>
+      <c r="AN7" s="13"/>
+      <c r="AO7" s="13"/>
+      <c r="AP7" s="13"/>
+      <c r="AQ7" s="13"/>
+      <c r="AR7" s="13"/>
+      <c r="AS7" s="13"/>
+      <c r="AT7" s="13"/>
+      <c r="AU7" s="13"/>
+      <c r="AV7" s="13"/>
+    </row>
+    <row r="8" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="11"/>
+      <c r="AE8" s="11"/>
+      <c r="AF8" s="10"/>
+      <c r="AG8" s="10"/>
+      <c r="AH8" s="13"/>
+      <c r="AI8" s="13"/>
+      <c r="AJ8" s="13"/>
+      <c r="AK8" s="13"/>
+      <c r="AL8" s="13"/>
+      <c r="AM8" s="13"/>
+      <c r="AN8" s="13"/>
+      <c r="AO8" s="13"/>
+      <c r="AP8" s="13"/>
+      <c r="AQ8" s="13"/>
+      <c r="AR8" s="13"/>
+      <c r="AS8" s="13"/>
+      <c r="AT8" s="13"/>
+      <c r="AU8" s="13"/>
+      <c r="AV8" s="13"/>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="14"/>
+      <c r="AB9" s="14"/>
+      <c r="AC9" s="14"/>
+      <c r="AD9" s="14"/>
+      <c r="AE9" s="14"/>
+      <c r="AF9" s="14"/>
+      <c r="AG9" s="14"/>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="10"/>
+      <c r="AC10" s="10"/>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="11"/>
+      <c r="AF10" s="10"/>
+      <c r="AG10" s="10"/>
+    </row>
+    <row r="11" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="10"/>
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="11"/>
+      <c r="AE11" s="11"/>
+      <c r="AF11" s="10"/>
+      <c r="AG11" s="10"/>
+    </row>
+    <row r="12" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="10"/>
+      <c r="AC12" s="10"/>
+      <c r="AD12" s="11"/>
+      <c r="AE12" s="11"/>
+      <c r="AF12" s="10"/>
+      <c r="AG12" s="10"/>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="10"/>
+      <c r="AC13" s="10"/>
+      <c r="AD13" s="11"/>
+      <c r="AE13" s="11"/>
+      <c r="AF13" s="10"/>
+      <c r="AG13" s="10"/>
+    </row>
+    <row r="14" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="10"/>
+      <c r="AC14" s="10"/>
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="11"/>
+      <c r="AF14" s="10"/>
+      <c r="AG14" s="10"/>
+    </row>
+    <row r="15" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="10"/>
+      <c r="AC15" s="10"/>
+      <c r="AD15" s="11"/>
+      <c r="AE15" s="11"/>
+      <c r="AF15" s="10"/>
+      <c r="AG15" s="10"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18"/>
+      <c r="U21" s="18"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="20"/>
+      <c r="U22" s="20"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R23" s="19"/>
+      <c r="S23" s="19"/>
+      <c r="T23" s="19"/>
+      <c r="U23" s="19"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="19"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="19"/>
+    </row>
+    <row r="26" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+    </row>
+    <row r="27" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="7">
+        <v>386</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7">
+        <v>386</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7">
+        <v>386</v>
+      </c>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7">
+        <v>386</v>
+      </c>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7">
+        <v>386</v>
+      </c>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R29" s="18"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="18"/>
+      <c r="U29" s="18"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+    </row>
+    <row r="31" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="19"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+    </row>
+    <row r="33" spans="18:21" x14ac:dyDescent="0.3">
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="19"/>
+    </row>
+    <row r="34" spans="18:21" x14ac:dyDescent="0.3">
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+    </row>
+    <row r="35" spans="18:21" x14ac:dyDescent="0.3">
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>